<commit_message>
Quest localization (not work)
- SkillManager.cs 등 FileRead에서 참조하는 함수 인자를 수정해두지 않아서 작동하지 않음. 다음 커밋으로 진행함.
</commit_message>
<xml_diff>
--- a/Assets/ExcelDatas/QuestTable.xlsx
+++ b/Assets/ExcelDatas/QuestTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Project-H9\Assets\ExcelDatas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB1FE5B3-0D16-4579-AA8D-A69CA97BD57E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2F8ED43-6C4D-42A3-BBCF-DF75E4B2550F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10260" yWindow="105" windowWidth="16950" windowHeight="15465" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="16950" windowHeight="15465" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -354,6 +354,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -362,12 +368,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -651,228 +651,228 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A37C4B6F-020E-46B5-A99A-D37C11C1CC21}">
   <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.125" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.125" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.25" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.375" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.875" style="9" customWidth="1"/>
-    <col min="6" max="6" width="9.5" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.25" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.25" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.125" style="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.875" style="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.875" style="9" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.625" style="9" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.125" style="9" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="50.125" style="10" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="9" style="9"/>
+    <col min="1" max="1" width="6.125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.125" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.25" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.375" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.875" style="6" customWidth="1"/>
+    <col min="6" max="6" width="9.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.25" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.25" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.125" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.875" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.875" style="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.625" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.125" style="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="50.125" style="7" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="9" t="s">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="M1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="N1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="O1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="P1" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2" s="9">
+      <c r="A2" s="6">
         <v>1</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="6">
         <v>1</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="6">
         <v>1</v>
       </c>
-      <c r="D2" s="9">
+      <c r="D2" s="6">
+        <v>2</v>
+      </c>
+      <c r="E2" s="6">
         <v>1</v>
       </c>
-      <c r="E2" s="9">
+      <c r="F2" s="6">
+        <v>0</v>
+      </c>
+      <c r="G2" s="6">
+        <v>0</v>
+      </c>
+      <c r="H2" s="7">
+        <v>0</v>
+      </c>
+      <c r="I2" s="6">
+        <v>-1</v>
+      </c>
+      <c r="J2" s="6">
         <v>1</v>
       </c>
-      <c r="F2" s="9">
-        <v>0</v>
-      </c>
-      <c r="G2" s="9">
-        <v>0</v>
-      </c>
-      <c r="H2" s="10">
-        <v>0</v>
-      </c>
-      <c r="I2" s="9">
+      <c r="K2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="6">
+        <v>100</v>
+      </c>
+      <c r="M2" s="6">
+        <v>100</v>
+      </c>
+      <c r="N2" s="6">
+        <v>0</v>
+      </c>
+      <c r="O2" s="6">
+        <v>0</v>
+      </c>
+      <c r="P2" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6">
+        <v>1</v>
+      </c>
+      <c r="C3" s="6">
+        <v>3</v>
+      </c>
+      <c r="D3" s="6">
+        <v>4</v>
+      </c>
+      <c r="E3" s="6">
+        <v>2</v>
+      </c>
+      <c r="F3" s="6">
+        <v>0</v>
+      </c>
+      <c r="G3" s="6">
+        <v>0</v>
+      </c>
+      <c r="H3" s="7">
+        <v>0</v>
+      </c>
+      <c r="I3" s="6">
         <v>-1</v>
       </c>
-      <c r="J2" s="9">
+      <c r="J3" s="6">
+        <v>2</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3" s="6">
+        <v>100</v>
+      </c>
+      <c r="M3" s="6">
+        <v>100</v>
+      </c>
+      <c r="N3" s="6">
+        <v>302</v>
+      </c>
+      <c r="O3" s="6">
+        <v>0</v>
+      </c>
+      <c r="P3" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4" s="6">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6">
         <v>1</v>
       </c>
-      <c r="K2" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="L2" s="9">
+      <c r="C4" s="6">
+        <v>5</v>
+      </c>
+      <c r="D4" s="6">
+        <v>6</v>
+      </c>
+      <c r="E4" s="6">
+        <v>3</v>
+      </c>
+      <c r="F4" s="6">
+        <v>0</v>
+      </c>
+      <c r="G4" s="6">
+        <v>0</v>
+      </c>
+      <c r="H4" s="7">
+        <v>0</v>
+      </c>
+      <c r="I4" s="6">
+        <v>-1</v>
+      </c>
+      <c r="J4" s="6">
+        <v>3</v>
+      </c>
+      <c r="K4" s="7">
+        <v>101</v>
+      </c>
+      <c r="L4" s="6">
         <v>100</v>
       </c>
-      <c r="M2" s="9">
+      <c r="M4" s="6">
         <v>100</v>
       </c>
-      <c r="N2" s="9">
-        <v>0</v>
-      </c>
-      <c r="O2" s="9">
-        <v>0</v>
-      </c>
-      <c r="P2" s="10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A3" s="9">
-        <v>2</v>
-      </c>
-      <c r="B3" s="9">
-        <v>1</v>
-      </c>
-      <c r="C3" s="9">
-        <v>2</v>
-      </c>
-      <c r="D3" s="9">
-        <v>2</v>
-      </c>
-      <c r="E3" s="9">
-        <v>2</v>
-      </c>
-      <c r="F3" s="9">
-        <v>0</v>
-      </c>
-      <c r="G3" s="9">
-        <v>0</v>
-      </c>
-      <c r="H3" s="10">
-        <v>0</v>
-      </c>
-      <c r="I3" s="9">
-        <v>-1</v>
-      </c>
-      <c r="J3" s="9">
-        <v>2</v>
-      </c>
-      <c r="K3" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="L3" s="9">
-        <v>100</v>
-      </c>
-      <c r="M3" s="9">
-        <v>100</v>
-      </c>
-      <c r="N3" s="9">
-        <v>302</v>
-      </c>
-      <c r="O3" s="9">
-        <v>0</v>
-      </c>
-      <c r="P3" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A4" s="9">
-        <v>3</v>
-      </c>
-      <c r="B4" s="9">
-        <v>1</v>
-      </c>
-      <c r="C4" s="9">
-        <v>3</v>
-      </c>
-      <c r="D4" s="9">
-        <v>3</v>
-      </c>
-      <c r="E4" s="9">
-        <v>3</v>
-      </c>
-      <c r="F4" s="9">
-        <v>0</v>
-      </c>
-      <c r="G4" s="9">
-        <v>0</v>
-      </c>
-      <c r="H4" s="10">
-        <v>0</v>
-      </c>
-      <c r="I4" s="9">
-        <v>-1</v>
-      </c>
-      <c r="J4" s="9">
-        <v>3</v>
-      </c>
-      <c r="K4" s="10">
-        <v>101</v>
-      </c>
-      <c r="L4" s="9">
-        <v>100</v>
-      </c>
-      <c r="M4" s="9">
-        <v>100</v>
-      </c>
-      <c r="N4" s="9">
-        <v>0</v>
-      </c>
-      <c r="O4" s="9">
+      <c r="N4" s="6">
+        <v>0</v>
+      </c>
+      <c r="O4" s="6">
         <v>22001</v>
       </c>
-      <c r="P4" s="10" t="s">
+      <c r="P4" s="7" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1054,7 +1054,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="8" t="s">
         <v>2</v>
       </c>
       <c r="B17" s="1">
@@ -1065,7 +1065,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="7"/>
+      <c r="A18" s="9"/>
       <c r="B18">
         <v>1</v>
       </c>
@@ -1074,7 +1074,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="8"/>
+      <c r="A19" s="10"/>
       <c r="B19" s="4">
         <v>2</v>
       </c>
@@ -1083,7 +1083,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B20" s="1">
@@ -1094,7 +1094,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="7"/>
+      <c r="A21" s="9"/>
       <c r="B21">
         <v>1</v>
       </c>
@@ -1103,7 +1103,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="7"/>
+      <c r="A22" s="9"/>
       <c r="B22">
         <v>2</v>
       </c>
@@ -1112,7 +1112,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="8"/>
+      <c r="A23" s="10"/>
       <c r="B23" s="4">
         <v>3</v>
       </c>

</xml_diff>